<commit_message>
ran resolve and classify+summarise steps after changes to mapping file
</commit_message>
<xml_diff>
--- a/01_analyses_mask-ONEland/results/SoIB_summaries.xlsx
+++ b/01_analyses_mask-ONEland/results/SoIB_summaries.xlsx
@@ -546,10 +546,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -559,10 +556,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>46</v>
-      </c>
-      <c r="C3">
-        <v>4.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -572,10 +566,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>220</v>
-      </c>
-      <c r="C4">
-        <v>23.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -585,10 +576,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>363</v>
-      </c>
-      <c r="C5">
-        <v>38.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -598,10 +586,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>178</v>
-      </c>
-      <c r="C6">
-        <v>18.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -611,10 +596,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>131</v>
-      </c>
-      <c r="C7">
-        <v>13.9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +737,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -795,73 +777,35 @@
         </is>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>46.2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Trend Different</t>
+          <t>IUCN</t>
         </is>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Range</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IUCN</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>23.1</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New files, changes to files and pipeline after bringing in memory optimized code.
Note that the results at this stage are incorrect because of a filtering issue that will be corrected in the next commit.
</commit_message>
<xml_diff>
--- a/01_analyses_mask-ONEland/results/SoIB_summaries.xlsx
+++ b/01_analyses_mask-ONEland/results/SoIB_summaries.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Range Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority Status" sheetId="3" r:id="rId3"/>
     <sheet name="Species qualification" sheetId="4" r:id="rId4"/>
-    <sheet name="High Priority break-up" sheetId="5" r:id="rId5"/>
+    <sheet name="Interannual update - High Pri" sheetId="5" r:id="rId5"/>
+    <sheet name="Major update - High Priority " sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -395,16 +396,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>37.5</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>41.4</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="3">
@@ -414,16 +415,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>45.8</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>27.6</v>
+        <v>36.8</v>
       </c>
     </row>
     <row r="4">
@@ -433,16 +434,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>16.7</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>27.6</v>
+        <v>42.1</v>
       </c>
     </row>
     <row r="5">
@@ -452,16 +453,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="6">
@@ -474,13 +475,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -490,10 +491,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -503,7 +504,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <v>69</v>
@@ -631,7 +632,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
@@ -641,7 +642,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4">
@@ -651,7 +652,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +688,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SoIB 2023 Assessment</t>
+          <t>SoIB Assessment</t>
         </is>
       </c>
       <c r="B2">
@@ -701,10 +702,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -717,7 +718,7 @@
         <v>49</v>
       </c>
       <c r="C4">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -736,6 +737,97 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Break-up</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>High Species (no.)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>High Species (perc.)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>New High Species (no.)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>New High Species (perc.)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Trend New</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>86</v>
+      </c>
+      <c r="C2">
+        <v>83.5</v>
+      </c>
+      <c r="D2">
+        <v>86</v>
+      </c>
+      <c r="E2">
+        <v>97.7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Trend Different</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IUCN</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>13.6</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>